<commit_message>
Bug Fixing on strategies. Corrected some values on Excel file.
</commit_message>
<xml_diff>
--- a/Part 4 - Implementation of evolutionary Axelrod Tournament/Additional Files/V_matrix.xlsx
+++ b/Part 4 - Implementation of evolutionary Axelrod Tournament/Additional Files/V_matrix.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gk_gi\Documents\σχολή\εργασίες\Θεωρία Παιγνίων\Part 4 - Implementation of evolutionary Axelrod Tournament\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gk_gi\Documents\σχολή\εργασίες\Θεωρία Παιγνίων\Part 4 - Implementation of evolutionary Axelrod Tournament\Additional Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1831B91-7C5F-49FB-9377-4EFA7C641E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CC5C0F-419A-4845-AB3A-A668DDD34263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -220,16 +220,16 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{4E79ECE5-AC8D-40F5-B022-C9C66CE5DD7F}" name="A/B" totalsRowLabel="Άθροισμα" dataDxfId="19" totalsRowDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{964D2443-2EB2-4228-B781-1AD9D2D1BE92}" name="ALL-C" dataDxfId="18" totalsRowDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{65F31C8A-0E4A-4DAA-8E7F-32477C2241F4}" name="ALL-D" dataDxfId="17" totalsRowDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{7E310E8C-0CA6-4C25-A90D-251570EE01D7}" name="TFT" dataDxfId="16" totalsRowDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{AAB4F91E-CB23-4DF6-A1AB-B198B36AC73C}" name="PER-CD" dataDxfId="15" totalsRowDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{38E8C1E4-63C0-4DF0-8A72-8A27F2DACCD4}" name="PER-DDC" dataDxfId="14" totalsRowDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{4F254969-EBFB-494C-84EE-B38DC71D2DEA}" name="PER-CCD" dataDxfId="13" totalsRowDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{98336271-ECEA-4C08-B92A-FD0B5C5FC9DF}" name="PER-CCCCD" dataDxfId="12" totalsRowDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{DE95F40A-26B8-44DF-9114-CBB8B1EDE3E2}" name="SOFT-M" dataDxfId="11" totalsRowDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{D9D665ED-F183-4091-94B7-87271AF8436C}" name="PROBER" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{4E79ECE5-AC8D-40F5-B022-C9C66CE5DD7F}" name="A/B" totalsRowLabel="Άθροισμα" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{964D2443-2EB2-4228-B781-1AD9D2D1BE92}" name="ALL-C" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{65F31C8A-0E4A-4DAA-8E7F-32477C2241F4}" name="ALL-D" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{7E310E8C-0CA6-4C25-A90D-251570EE01D7}" name="TFT" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{AAB4F91E-CB23-4DF6-A1AB-B198B36AC73C}" name="PER-CD" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{38E8C1E4-63C0-4DF0-8A72-8A27F2DACCD4}" name="PER-DDC" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{4F254969-EBFB-494C-84EE-B38DC71D2DEA}" name="PER-CCD" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{98336271-ECEA-4C08-B92A-FD0B5C5FC9DF}" name="PER-CCCCD" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{DE95F40A-26B8-44DF-9114-CBB8B1EDE3E2}" name="SOFT-M" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{D9D665ED-F183-4091-94B7-87271AF8436C}" name="PROBER" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -501,7 +501,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -558,10 +558,10 @@
         <v>1500</v>
       </c>
       <c r="F2" s="1">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="G2" s="1">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="H2" s="1">
         <v>2400</v>
@@ -654,7 +654,7 @@
         <v>2000</v>
       </c>
       <c r="F5" s="1">
-        <v>1001</v>
+        <v>1665</v>
       </c>
       <c r="G5" s="1">
         <v>2835</v>
@@ -750,7 +750,7 @@
         <v>1800</v>
       </c>
       <c r="F8" s="1">
-        <v>1064</v>
+        <v>1265</v>
       </c>
       <c r="G8" s="1">
         <v>2335</v>
@@ -785,7 +785,7 @@
         <v>2331</v>
       </c>
       <c r="G9" s="1">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="H9" s="1">
         <v>2400</v>
@@ -811,7 +811,7 @@
         <v>2999</v>
       </c>
       <c r="E10" s="1">
-        <v>2503</v>
+        <v>2498</v>
       </c>
       <c r="F10" s="1">
         <v>1996</v>

</xml_diff>